<commit_message>
Improve 118 bus system
Add IBR into the system.
</commit_message>
<xml_diff>
--- a/Simulation118Bus/Data118Bus.xlsx
+++ b/Simulation118Bus/Data118Bus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Simulation118Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE18C27-C8FF-41AC-ACA5-6FFA7E0FFFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE260AA-DE9F-41C4-9F2E-5C484EC2A135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -5160,8 +5160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" activeCellId="31" sqref="B7 B9 B11 B13 B15:B16 B18:B19 B22:B25 B30:B32 B35 B37 B39:B41 B43 B45:B47 B49:B50 B52:B55 B59:B60 B62 B65:B66 B69:B70 B73 B77 B80:B81 B83:B86 B88 B90 B95:B100 B103:B104 B108 B110:B111 B116:B117 B119:B120 B4:B5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -5209,7 +5209,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E3" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5251,7 +5251,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E6" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5274,20 +5274,29 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>50</v>
-      </c>
-      <c r="D8" s="9">
-        <v>50</v>
-      </c>
-      <c r="E8" s="9">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>2.5</v>
+      </c>
+      <c r="D8">
+        <v>2E-3</v>
+      </c>
+      <c r="E8">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F8" s="9">
-        <f>E8/5</f>
-        <v>1E-3</v>
+      <c r="F8">
+        <f t="shared" ref="F8" si="0">E8/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
@@ -5309,7 +5318,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E10" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5332,20 +5341,29 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9">
-        <v>50</v>
-      </c>
-      <c r="D12" s="9">
-        <v>50</v>
-      </c>
-      <c r="E12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>2.5</v>
+      </c>
+      <c r="D12">
+        <v>2E-3</v>
+      </c>
+      <c r="E12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F12" s="9">
-        <f>E12/5</f>
-        <v>1E-3</v>
+      <c r="F12">
+        <f t="shared" ref="F12" si="1">E12/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
@@ -5361,20 +5379,29 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>50</v>
-      </c>
-      <c r="D14" s="9">
-        <v>50</v>
-      </c>
-      <c r="E14" s="9">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>2.5</v>
+      </c>
+      <c r="D14">
+        <v>2E-3</v>
+      </c>
+      <c r="E14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F14" s="9">
-        <f>E14/5</f>
-        <v>1E-3</v>
+      <c r="F14">
+        <f t="shared" ref="F14" si="2">E14/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
@@ -5393,7 +5420,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -5404,7 +5431,7 @@
         <v>50</v>
       </c>
       <c r="D17" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E17" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5414,7 +5441,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="7">
         <v>16</v>
       </c>
@@ -5422,7 +5449,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -5430,7 +5457,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="7">
         <v>18</v>
       </c>
@@ -5441,7 +5468,7 @@
         <v>50</v>
       </c>
       <c r="D20" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E20" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5451,28 +5478,37 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="7">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
-        <v>50</v>
-      </c>
-      <c r="D21" s="9">
-        <v>50</v>
-      </c>
-      <c r="E21" s="9">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>2.5</v>
+      </c>
+      <c r="D21">
+        <v>2E-3</v>
+      </c>
+      <c r="E21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F21" s="9">
-        <f>E21/5</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F21">
+        <f t="shared" ref="F21" si="3">E21/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="7">
         <v>20</v>
       </c>
@@ -5480,7 +5516,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="7">
         <v>21</v>
       </c>
@@ -5488,7 +5524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="7">
         <v>22</v>
       </c>
@@ -5496,7 +5532,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="7">
         <v>23</v>
       </c>
@@ -5504,7 +5540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="7">
         <v>24</v>
       </c>
@@ -5515,17 +5551,17 @@
         <v>50</v>
       </c>
       <c r="D26" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E26" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" ref="F26:F29" si="0">E26/5</f>
+        <f t="shared" ref="F26:F29" si="4">E26/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="7">
         <v>25</v>
       </c>
@@ -5536,59 +5572,77 @@
         <v>50</v>
       </c>
       <c r="D27" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E27" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="7">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28" s="9">
-        <v>50</v>
-      </c>
-      <c r="D28" s="9">
-        <v>50</v>
-      </c>
-      <c r="E28" s="9">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>2.5</v>
+      </c>
+      <c r="D28">
+        <v>2E-3</v>
+      </c>
+      <c r="E28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F28" s="9">
-        <f t="shared" si="0"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F28">
+        <f t="shared" ref="F28" si="5">E28/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="7">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" s="9">
-        <v>50</v>
-      </c>
-      <c r="D29" s="9">
-        <v>50</v>
-      </c>
-      <c r="E29" s="9">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>2.5</v>
+      </c>
+      <c r="D29">
+        <v>2E-3</v>
+      </c>
+      <c r="E29">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F29" s="9">
-        <f t="shared" si="0"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F29">
+        <f t="shared" ref="F29" si="6">E29/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="7">
         <v>28</v>
       </c>
@@ -5596,7 +5650,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
         <v>29</v>
       </c>
@@ -5604,7 +5658,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="7">
         <v>30</v>
       </c>
@@ -5612,7 +5666,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="7">
         <v>31</v>
       </c>
@@ -5623,38 +5677,47 @@
         <v>50</v>
       </c>
       <c r="D33" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E33" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" ref="F33:F34" si="1">E33/5</f>
+        <f t="shared" ref="F33:F34" si="7">E33/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="7">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34" s="9">
-        <v>50</v>
-      </c>
-      <c r="D34" s="9">
-        <v>50</v>
-      </c>
-      <c r="E34" s="9">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>2.5</v>
+      </c>
+      <c r="D34">
+        <v>2E-3</v>
+      </c>
+      <c r="E34">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F34" s="9">
-        <f t="shared" si="1"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F34">
+        <f t="shared" ref="F34" si="8">E34/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>10</v>
+      </c>
+      <c r="I34">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="7">
         <v>33</v>
       </c>
@@ -5662,7 +5725,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="7">
         <v>34</v>
       </c>
@@ -5673,7 +5736,7 @@
         <v>50</v>
       </c>
       <c r="D36" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E36" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5683,7 +5746,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="7">
         <v>35</v>
       </c>
@@ -5691,7 +5754,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="7">
         <v>36</v>
       </c>
@@ -5702,7 +5765,7 @@
         <v>50</v>
       </c>
       <c r="D38" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E38" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5712,7 +5775,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="7">
         <v>37</v>
       </c>
@@ -5720,7 +5783,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="7">
         <v>38</v>
       </c>
@@ -5728,7 +5791,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="7">
         <v>39</v>
       </c>
@@ -5736,7 +5799,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="7">
         <v>40</v>
       </c>
@@ -5747,7 +5810,7 @@
         <v>50</v>
       </c>
       <c r="D42" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E42" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5757,7 +5820,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="7">
         <v>41</v>
       </c>
@@ -5765,28 +5828,37 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="7">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44" s="9">
-        <v>50</v>
-      </c>
-      <c r="D44" s="9">
-        <v>50</v>
-      </c>
-      <c r="E44" s="9">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>2.5</v>
+      </c>
+      <c r="D44">
+        <v>2E-3</v>
+      </c>
+      <c r="E44">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F44" s="9">
-        <f>E44/5</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F44">
+        <f t="shared" ref="F44" si="9">E44/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G44">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <v>10</v>
+      </c>
+      <c r="I44">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="7">
         <v>43</v>
       </c>
@@ -5794,7 +5866,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="7">
         <v>44</v>
       </c>
@@ -5802,7 +5874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="7">
         <v>45</v>
       </c>
@@ -5810,7 +5882,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" s="7">
         <v>46</v>
       </c>
@@ -5821,7 +5893,7 @@
         <v>50</v>
       </c>
       <c r="D48" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E48" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5831,7 +5903,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" s="7">
         <v>47</v>
       </c>
@@ -5839,7 +5911,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" s="7">
         <v>48</v>
       </c>
@@ -5847,7 +5919,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" s="7">
         <v>49</v>
       </c>
@@ -5858,7 +5930,7 @@
         <v>50</v>
       </c>
       <c r="D51" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E51" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5868,7 +5940,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" s="7">
         <v>50</v>
       </c>
@@ -5876,7 +5948,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" s="7">
         <v>51</v>
       </c>
@@ -5884,7 +5956,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" s="7">
         <v>52</v>
       </c>
@@ -5892,7 +5964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" s="7">
         <v>53</v>
       </c>
@@ -5900,7 +5972,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A56" s="7">
         <v>54</v>
       </c>
@@ -5911,17 +5983,17 @@
         <v>50</v>
       </c>
       <c r="D56" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E56" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F56" s="9">
-        <f t="shared" ref="F56:F58" si="2">E56/5</f>
+        <f t="shared" ref="F56:F58" si="10">E56/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A57" s="7">
         <v>55</v>
       </c>
@@ -5932,38 +6004,47 @@
         <v>50</v>
       </c>
       <c r="D57" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E57" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A58" s="7">
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58" s="9">
-        <v>50</v>
-      </c>
-      <c r="D58" s="9">
-        <v>50</v>
-      </c>
-      <c r="E58" s="9">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>2.5</v>
+      </c>
+      <c r="D58">
+        <v>2E-3</v>
+      </c>
+      <c r="E58">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F58" s="9">
-        <f t="shared" si="2"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F58">
+        <f t="shared" ref="F58" si="11">E58/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G58">
+        <v>10</v>
+      </c>
+      <c r="H58">
+        <v>10</v>
+      </c>
+      <c r="I58">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A59" s="7">
         <v>57</v>
       </c>
@@ -5971,7 +6052,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A60" s="7">
         <v>58</v>
       </c>
@@ -5979,7 +6060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A61" s="7">
         <v>59</v>
       </c>
@@ -5990,7 +6071,7 @@
         <v>50</v>
       </c>
       <c r="D61" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E61" s="9">
         <v>5.0000000000000001E-3</v>
@@ -6000,7 +6081,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A62" s="7">
         <v>60</v>
       </c>
@@ -6008,7 +6089,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A63" s="7">
         <v>61</v>
       </c>
@@ -6019,38 +6100,47 @@
         <v>50</v>
       </c>
       <c r="D63" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E63" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F63" s="9">
-        <f t="shared" ref="F63:F64" si="3">E63/5</f>
+        <f t="shared" ref="F63:F64" si="12">E63/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A64" s="7">
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0</v>
-      </c>
-      <c r="C64" s="9">
-        <v>50</v>
-      </c>
-      <c r="D64" s="9">
-        <v>50</v>
-      </c>
-      <c r="E64" s="9">
+        <v>10</v>
+      </c>
+      <c r="C64">
+        <v>2.5</v>
+      </c>
+      <c r="D64">
+        <v>2E-3</v>
+      </c>
+      <c r="E64">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F64" s="9">
-        <f t="shared" si="3"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F64">
+        <f t="shared" ref="F64" si="13">E64/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G64">
+        <v>10</v>
+      </c>
+      <c r="H64">
+        <v>10</v>
+      </c>
+      <c r="I64">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A65" s="7">
         <v>63</v>
       </c>
@@ -6058,7 +6148,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A66" s="7">
         <v>64</v>
       </c>
@@ -6066,7 +6156,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A67" s="7">
         <v>65</v>
       </c>
@@ -6077,38 +6167,47 @@
         <v>50</v>
       </c>
       <c r="D67" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E67" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F67" s="9">
-        <f t="shared" ref="F67:F68" si="4">E67/5</f>
+        <f t="shared" ref="F67:F68" si="14">E67/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A68" s="7">
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68" s="9">
-        <v>50</v>
-      </c>
-      <c r="D68" s="9">
-        <v>50</v>
-      </c>
-      <c r="E68" s="9">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>2.5</v>
+      </c>
+      <c r="D68">
+        <v>2E-3</v>
+      </c>
+      <c r="E68">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F68" s="9">
-        <f t="shared" si="4"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F68">
+        <f t="shared" ref="F68" si="15">E68/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G68">
+        <v>10</v>
+      </c>
+      <c r="H68">
+        <v>10</v>
+      </c>
+      <c r="I68">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A69" s="7">
         <v>67</v>
       </c>
@@ -6116,7 +6215,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A70" s="7">
         <v>68</v>
       </c>
@@ -6124,7 +6223,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A71" s="7">
         <v>69</v>
       </c>
@@ -6135,38 +6234,47 @@
         <v>50</v>
       </c>
       <c r="D71" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E71" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F71" s="9">
-        <f t="shared" ref="F71:F72" si="5">E71/5</f>
+        <f t="shared" ref="F71:F72" si="16">E71/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A72" s="7">
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0</v>
-      </c>
-      <c r="C72" s="9">
-        <v>50</v>
-      </c>
-      <c r="D72" s="9">
-        <v>50</v>
-      </c>
-      <c r="E72" s="9">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>2.5</v>
+      </c>
+      <c r="D72">
+        <v>2E-3</v>
+      </c>
+      <c r="E72">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F72" s="9">
-        <f t="shared" si="5"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F72">
+        <f t="shared" ref="F72" si="17">E72/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G72">
+        <v>10</v>
+      </c>
+      <c r="H72">
+        <v>10</v>
+      </c>
+      <c r="I72">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A73" s="7">
         <v>71</v>
       </c>
@@ -6174,7 +6282,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A74" s="7">
         <v>72</v>
       </c>
@@ -6185,17 +6293,17 @@
         <v>50</v>
       </c>
       <c r="D74" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E74" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F74" s="9">
-        <f t="shared" ref="F74:F76" si="6">E74/5</f>
+        <f t="shared" ref="F74:F76" si="18">E74/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A75" s="7">
         <v>73</v>
       </c>
@@ -6206,38 +6314,47 @@
         <v>50</v>
       </c>
       <c r="D75" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E75" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F75" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A76" s="7">
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76" s="9">
-        <v>50</v>
-      </c>
-      <c r="D76" s="9">
-        <v>50</v>
-      </c>
-      <c r="E76" s="9">
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <v>2.5</v>
+      </c>
+      <c r="D76">
+        <v>2E-3</v>
+      </c>
+      <c r="E76">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F76" s="9">
-        <f t="shared" si="6"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F76">
+        <f t="shared" ref="F76" si="19">E76/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G76">
+        <v>10</v>
+      </c>
+      <c r="H76">
+        <v>10</v>
+      </c>
+      <c r="I76">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A77" s="7">
         <v>75</v>
       </c>
@@ -6245,7 +6362,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A78" s="7">
         <v>76</v>
       </c>
@@ -6256,38 +6373,47 @@
         <v>50</v>
       </c>
       <c r="D78" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E78" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F78" s="9">
-        <f t="shared" ref="F78:F79" si="7">E78/5</f>
+        <f t="shared" ref="F78:F79" si="20">E78/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A79" s="7">
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0</v>
-      </c>
-      <c r="C79" s="9">
-        <v>50</v>
-      </c>
-      <c r="D79" s="9">
-        <v>50</v>
-      </c>
-      <c r="E79" s="9">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>2.5</v>
+      </c>
+      <c r="D79">
+        <v>2E-3</v>
+      </c>
+      <c r="E79">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F79" s="9">
-        <f t="shared" si="7"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F79">
+        <f t="shared" ref="F79" si="21">E79/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G79">
+        <v>10</v>
+      </c>
+      <c r="H79">
+        <v>10</v>
+      </c>
+      <c r="I79">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A80" s="7">
         <v>78</v>
       </c>
@@ -6295,7 +6421,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A81" s="7">
         <v>79</v>
       </c>
@@ -6303,7 +6429,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A82" s="7">
         <v>80</v>
       </c>
@@ -6314,7 +6440,7 @@
         <v>50</v>
       </c>
       <c r="D82" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E82" s="9">
         <v>5.0000000000000001E-3</v>
@@ -6324,7 +6450,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A83" s="7">
         <v>81</v>
       </c>
@@ -6332,7 +6458,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A84" s="7">
         <v>82</v>
       </c>
@@ -6340,7 +6466,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A85" s="7">
         <v>83</v>
       </c>
@@ -6348,7 +6474,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A86" s="7">
         <v>84</v>
       </c>
@@ -6356,28 +6482,37 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A87" s="7">
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0</v>
-      </c>
-      <c r="C87" s="9">
-        <v>50</v>
-      </c>
-      <c r="D87" s="9">
-        <v>50</v>
-      </c>
-      <c r="E87" s="9">
+        <v>10</v>
+      </c>
+      <c r="C87">
+        <v>2.5</v>
+      </c>
+      <c r="D87">
+        <v>2E-3</v>
+      </c>
+      <c r="E87">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F87" s="9">
-        <f>E87/5</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F87">
+        <f t="shared" ref="F87" si="22">E87/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G87">
+        <v>10</v>
+      </c>
+      <c r="H87">
+        <v>10</v>
+      </c>
+      <c r="I87">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A88" s="7">
         <v>86</v>
       </c>
@@ -6385,7 +6520,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A89" s="7">
         <v>87</v>
       </c>
@@ -6406,7 +6541,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A90" s="7">
         <v>88</v>
       </c>
@@ -6414,7 +6549,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A91" s="7">
         <v>89</v>
       </c>
@@ -6431,11 +6566,11 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F91" s="9">
-        <f t="shared" ref="F91:F94" si="8">E91/5</f>
+        <f t="shared" ref="F91:F94" si="23">E91/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A92" s="7">
         <v>90</v>
       </c>
@@ -6452,53 +6587,71 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F92" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="23"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A93" s="7">
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0</v>
-      </c>
-      <c r="C93" s="9">
-        <v>50</v>
-      </c>
-      <c r="D93" s="9">
-        <v>50</v>
-      </c>
-      <c r="E93" s="9">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>2.5</v>
+      </c>
+      <c r="D93">
+        <v>2E-3</v>
+      </c>
+      <c r="E93">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F93" s="9">
-        <f t="shared" si="8"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F93">
+        <f t="shared" ref="F93" si="24">E93/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G93">
+        <v>10</v>
+      </c>
+      <c r="H93">
+        <v>10</v>
+      </c>
+      <c r="I93">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A94" s="7">
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0</v>
-      </c>
-      <c r="C94" s="9">
-        <v>50</v>
-      </c>
-      <c r="D94" s="9">
-        <v>50</v>
-      </c>
-      <c r="E94" s="9">
+        <v>10</v>
+      </c>
+      <c r="C94">
+        <v>2.5</v>
+      </c>
+      <c r="D94">
+        <v>2E-3</v>
+      </c>
+      <c r="E94">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F94" s="9">
-        <f t="shared" si="8"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F94">
+        <f t="shared" ref="F94" si="25">E94/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G94">
+        <v>10</v>
+      </c>
+      <c r="H94">
+        <v>10</v>
+      </c>
+      <c r="I94">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A95" s="7">
         <v>93</v>
       </c>
@@ -6506,7 +6659,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A96" s="7">
         <v>94</v>
       </c>
@@ -6514,7 +6667,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A97" s="7">
         <v>95</v>
       </c>
@@ -6522,7 +6675,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A98" s="7">
         <v>96</v>
       </c>
@@ -6530,7 +6683,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A99" s="7">
         <v>97</v>
       </c>
@@ -6538,7 +6691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A100" s="7">
         <v>98</v>
       </c>
@@ -6546,7 +6699,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A101" s="7">
         <v>99</v>
       </c>
@@ -6563,11 +6716,11 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F101" s="9">
-        <f t="shared" ref="F101:F102" si="9">E101/5</f>
+        <f t="shared" ref="F101:F102" si="26">E101/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A102" s="7">
         <v>100</v>
       </c>
@@ -6584,11 +6737,11 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F102" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="26"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A103" s="7">
         <v>101</v>
       </c>
@@ -6596,7 +6749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A104" s="7">
         <v>102</v>
       </c>
@@ -6604,7 +6757,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A105" s="7">
         <v>103</v>
       </c>
@@ -6621,11 +6774,11 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F105" s="9">
-        <f t="shared" ref="F105:F107" si="10">E105/5</f>
+        <f t="shared" ref="F105:F107" si="27">E105/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A106" s="7">
         <v>104</v>
       </c>
@@ -6642,32 +6795,41 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F106" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="27"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A107" s="7">
         <v>105</v>
       </c>
       <c r="B107">
-        <v>0</v>
-      </c>
-      <c r="C107" s="9">
-        <v>50</v>
-      </c>
-      <c r="D107" s="9">
-        <v>50</v>
-      </c>
-      <c r="E107" s="9">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>2.5</v>
+      </c>
+      <c r="D107">
+        <v>2E-3</v>
+      </c>
+      <c r="E107">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F107" s="9">
-        <f t="shared" si="10"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F107">
+        <f t="shared" ref="F107" si="28">E107/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G107">
+        <v>10</v>
+      </c>
+      <c r="H107">
+        <v>10</v>
+      </c>
+      <c r="I107">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A108" s="7">
         <v>106</v>
       </c>
@@ -6675,7 +6837,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A109" s="7">
         <v>107</v>
       </c>
@@ -6696,7 +6858,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A110" s="7">
         <v>108</v>
       </c>
@@ -6704,7 +6866,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A111" s="7">
         <v>109</v>
       </c>
@@ -6712,7 +6874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A112" s="7">
         <v>110</v>
       </c>
@@ -6729,11 +6891,11 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F112" s="9">
-        <f t="shared" ref="F112:F115" si="11">E112/5</f>
+        <f t="shared" ref="F112:F115" si="29">E112/5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A113" s="7">
         <v>111</v>
       </c>
@@ -6750,53 +6912,71 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F113" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="29"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A114" s="7">
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0</v>
-      </c>
-      <c r="C114" s="9">
-        <v>50</v>
-      </c>
-      <c r="D114" s="9">
-        <v>50</v>
-      </c>
-      <c r="E114" s="9">
+        <v>10</v>
+      </c>
+      <c r="C114">
+        <v>2.5</v>
+      </c>
+      <c r="D114">
+        <v>2E-3</v>
+      </c>
+      <c r="E114">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F114" s="9">
-        <f t="shared" si="11"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F114">
+        <f t="shared" ref="F114" si="30">E114/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G114">
+        <v>10</v>
+      </c>
+      <c r="H114">
+        <v>10</v>
+      </c>
+      <c r="I114">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A115" s="7">
         <v>113</v>
       </c>
       <c r="B115">
-        <v>0</v>
-      </c>
-      <c r="C115" s="9">
-        <v>50</v>
-      </c>
-      <c r="D115" s="9">
-        <v>50</v>
-      </c>
-      <c r="E115" s="9">
+        <v>10</v>
+      </c>
+      <c r="C115">
+        <v>2.5</v>
+      </c>
+      <c r="D115">
+        <v>2E-3</v>
+      </c>
+      <c r="E115">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F115" s="9">
-        <f t="shared" si="11"/>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F115">
+        <f t="shared" ref="F115" si="31">E115/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G115">
+        <v>10</v>
+      </c>
+      <c r="H115">
+        <v>10</v>
+      </c>
+      <c r="I115">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A116" s="7">
         <v>114</v>
       </c>
@@ -6804,7 +6984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A117" s="7">
         <v>115</v>
       </c>
@@ -6812,28 +6992,37 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A118" s="7">
         <v>116</v>
       </c>
       <c r="B118">
-        <v>0</v>
-      </c>
-      <c r="C118" s="9">
-        <v>50</v>
-      </c>
-      <c r="D118" s="9">
-        <v>50</v>
-      </c>
-      <c r="E118" s="9">
+        <v>10</v>
+      </c>
+      <c r="C118">
+        <v>2.5</v>
+      </c>
+      <c r="D118">
+        <v>2E-3</v>
+      </c>
+      <c r="E118">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F118" s="9">
-        <f>E118/5</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F118">
+        <f t="shared" ref="F118" si="32">E118/10</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G118">
+        <v>10</v>
+      </c>
+      <c r="H118">
+        <v>10</v>
+      </c>
+      <c r="I118">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A119" s="7">
         <v>117</v>
       </c>
@@ -6841,7 +7030,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A120" s="7">
         <v>118</v>
       </c>
@@ -6860,8 +7049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
   <dimension ref="A1:G191"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -11284,7 +11473,7 @@
       </c>
       <c r="B2" s="1">
         <f>B3*500</f>
-        <v>25000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -11292,7 +11481,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -11323,7 +11512,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -11390,7 +11579,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Test 118 bus system
</commit_message>
<xml_diff>
--- a/Simulation118Bus/Data118Bus.xlsx
+++ b/Simulation118Bus/Data118Bus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Simulation118Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE260AA-DE9F-41C4-9F2E-5C484EC2A135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD048A00-2D48-4EC6-A78E-3E6B3D964284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5160,8 +5160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -5209,7 +5209,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E3" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5251,13 +5251,12 @@
         <v>50</v>
       </c>
       <c r="D6" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E6" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F6" s="9">
-        <f>E6/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -5280,20 +5279,19 @@
         <v>2.5</v>
       </c>
       <c r="D8">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E8">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8" si="0">E8/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I8">
         <v>400</v>
@@ -5318,7 +5316,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E10" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5347,20 +5345,19 @@
         <v>2.5</v>
       </c>
       <c r="D12">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E12">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12" si="1">E12/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <v>400</v>
@@ -5385,20 +5382,19 @@
         <v>2.5</v>
       </c>
       <c r="D14">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E14">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14" si="2">E14/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I14">
         <v>400</v>
@@ -5431,7 +5427,7 @@
         <v>50</v>
       </c>
       <c r="D17" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E17" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5468,7 +5464,7 @@
         <v>50</v>
       </c>
       <c r="D20" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E20" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5489,20 +5485,19 @@
         <v>2.5</v>
       </c>
       <c r="D21">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E21">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21" si="3">E21/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I21">
         <v>400</v>
@@ -5551,13 +5546,13 @@
         <v>50</v>
       </c>
       <c r="D26" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E26" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" ref="F26:F29" si="4">E26/5</f>
+        <f t="shared" ref="F26:F27" si="0">E26/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -5572,13 +5567,13 @@
         <v>50</v>
       </c>
       <c r="D27" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E27" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -5593,20 +5588,19 @@
         <v>2.5</v>
       </c>
       <c r="D28">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E28">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28" si="5">E28/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G28">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H28">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I28">
         <v>400</v>
@@ -5623,20 +5617,19 @@
         <v>2.5</v>
       </c>
       <c r="D29">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E29">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29" si="6">E29/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I29">
         <v>400</v>
@@ -5677,13 +5670,13 @@
         <v>50</v>
       </c>
       <c r="D33" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E33" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" ref="F33:F34" si="7">E33/5</f>
+        <f t="shared" ref="F33" si="1">E33/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -5698,20 +5691,19 @@
         <v>2.5</v>
       </c>
       <c r="D34">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E34">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34" si="8">E34/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H34">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I34">
         <v>400</v>
@@ -5736,7 +5728,7 @@
         <v>50</v>
       </c>
       <c r="D36" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E36" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5765,7 +5757,7 @@
         <v>50</v>
       </c>
       <c r="D38" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E38" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5810,7 +5802,7 @@
         <v>50</v>
       </c>
       <c r="D42" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E42" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5839,20 +5831,19 @@
         <v>2.5</v>
       </c>
       <c r="D44">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E44">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F44">
-        <f t="shared" ref="F44" si="9">E44/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G44">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H44">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I44">
         <v>400</v>
@@ -5893,7 +5884,7 @@
         <v>50</v>
       </c>
       <c r="D48" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E48" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5930,7 +5921,7 @@
         <v>50</v>
       </c>
       <c r="D51" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E51" s="9">
         <v>5.0000000000000001E-3</v>
@@ -5983,13 +5974,13 @@
         <v>50</v>
       </c>
       <c r="D56" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E56" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F56" s="9">
-        <f t="shared" ref="F56:F58" si="10">E56/5</f>
+        <f t="shared" ref="F56:F57" si="2">E56/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6004,13 +5995,13 @@
         <v>50</v>
       </c>
       <c r="D57" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E57" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -6025,20 +6016,19 @@
         <v>2.5</v>
       </c>
       <c r="D58">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E58">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F58">
-        <f t="shared" ref="F58" si="11">E58/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G58">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H58">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I58">
         <v>400</v>
@@ -6071,7 +6061,7 @@
         <v>50</v>
       </c>
       <c r="D61" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E61" s="9">
         <v>5.0000000000000001E-3</v>
@@ -6100,13 +6090,13 @@
         <v>50</v>
       </c>
       <c r="D63" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E63" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F63" s="9">
-        <f t="shared" ref="F63:F64" si="12">E63/5</f>
+        <f t="shared" ref="F63" si="3">E63/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6121,20 +6111,19 @@
         <v>2.5</v>
       </c>
       <c r="D64">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E64">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F64">
-        <f t="shared" ref="F64" si="13">E64/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G64">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H64">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I64">
         <v>400</v>
@@ -6167,13 +6156,13 @@
         <v>50</v>
       </c>
       <c r="D67" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E67" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F67" s="9">
-        <f t="shared" ref="F67:F68" si="14">E67/5</f>
+        <f t="shared" ref="F67" si="4">E67/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6188,20 +6177,19 @@
         <v>2.5</v>
       </c>
       <c r="D68">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E68">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68" si="15">E68/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G68">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H68">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I68">
         <v>400</v>
@@ -6234,13 +6222,13 @@
         <v>50</v>
       </c>
       <c r="D71" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E71" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F71" s="9">
-        <f t="shared" ref="F71:F72" si="16">E71/5</f>
+        <f t="shared" ref="F71" si="5">E71/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6255,20 +6243,19 @@
         <v>2.5</v>
       </c>
       <c r="D72">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E72">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F72">
-        <f t="shared" ref="F72" si="17">E72/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G72">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H72">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I72">
         <v>400</v>
@@ -6293,13 +6280,13 @@
         <v>50</v>
       </c>
       <c r="D74" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E74" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F74" s="9">
-        <f t="shared" ref="F74:F76" si="18">E74/5</f>
+        <f t="shared" ref="F74:F75" si="6">E74/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6314,13 +6301,13 @@
         <v>50</v>
       </c>
       <c r="D75" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E75" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F75" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -6335,20 +6322,19 @@
         <v>2.5</v>
       </c>
       <c r="D76">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E76">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F76">
-        <f t="shared" ref="F76" si="19">E76/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G76">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H76">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I76">
         <v>400</v>
@@ -6373,13 +6359,13 @@
         <v>50</v>
       </c>
       <c r="D78" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E78" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F78" s="9">
-        <f t="shared" ref="F78:F79" si="20">E78/5</f>
+        <f t="shared" ref="F78" si="7">E78/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6394,20 +6380,19 @@
         <v>2.5</v>
       </c>
       <c r="D79">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E79">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F79">
-        <f t="shared" ref="F79" si="21">E79/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G79">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H79">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I79">
         <v>400</v>
@@ -6440,7 +6425,7 @@
         <v>50</v>
       </c>
       <c r="D82" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E82" s="9">
         <v>5.0000000000000001E-3</v>
@@ -6493,14 +6478,13 @@
         <v>2.5</v>
       </c>
       <c r="D87">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E87">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F87">
-        <f t="shared" ref="F87" si="22">E87/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G87">
         <v>10</v>
@@ -6531,7 +6515,7 @@
         <v>50</v>
       </c>
       <c r="D89" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E89" s="9">
         <v>5.0000000000000001E-3</v>
@@ -6560,13 +6544,13 @@
         <v>50</v>
       </c>
       <c r="D91" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E91" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F91" s="9">
-        <f t="shared" ref="F91:F94" si="23">E91/5</f>
+        <f t="shared" ref="F91:F92" si="8">E91/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6581,13 +6565,13 @@
         <v>50</v>
       </c>
       <c r="D92" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E92" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F92" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="8"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -6602,14 +6586,13 @@
         <v>2.5</v>
       </c>
       <c r="D93">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E93">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F93">
-        <f t="shared" ref="F93" si="24">E93/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G93">
         <v>10</v>
@@ -6632,14 +6615,13 @@
         <v>2.5</v>
       </c>
       <c r="D94">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E94">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F94">
-        <f t="shared" ref="F94" si="25">E94/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G94">
         <v>10</v>
@@ -6710,13 +6692,13 @@
         <v>50</v>
       </c>
       <c r="D101" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E101" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F101" s="9">
-        <f t="shared" ref="F101:F102" si="26">E101/5</f>
+        <f t="shared" ref="F101:F102" si="9">E101/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6731,13 +6713,13 @@
         <v>50</v>
       </c>
       <c r="D102" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E102" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F102" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -6768,13 +6750,13 @@
         <v>50</v>
       </c>
       <c r="D105" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E105" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F105" s="9">
-        <f t="shared" ref="F105:F107" si="27">E105/5</f>
+        <f t="shared" ref="F105:F106" si="10">E105/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6789,13 +6771,13 @@
         <v>50</v>
       </c>
       <c r="D106" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E106" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F106" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="10"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -6810,14 +6792,13 @@
         <v>2.5</v>
       </c>
       <c r="D107">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E107">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F107">
-        <f t="shared" ref="F107" si="28">E107/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G107">
         <v>10</v>
@@ -6848,7 +6829,7 @@
         <v>50</v>
       </c>
       <c r="D109" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E109" s="9">
         <v>5.0000000000000001E-3</v>
@@ -6885,13 +6866,13 @@
         <v>50</v>
       </c>
       <c r="D112" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E112" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F112" s="9">
-        <f t="shared" ref="F112:F115" si="29">E112/5</f>
+        <f t="shared" ref="F112:F113" si="11">E112/5</f>
         <v>1E-3</v>
       </c>
     </row>
@@ -6906,13 +6887,13 @@
         <v>50</v>
       </c>
       <c r="D113" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E113" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F113" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -6927,14 +6908,13 @@
         <v>2.5</v>
       </c>
       <c r="D114">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E114">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F114">
-        <f t="shared" ref="F114" si="30">E114/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G114">
         <v>10</v>
@@ -6957,14 +6937,13 @@
         <v>2.5</v>
       </c>
       <c r="D115">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E115">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F115">
-        <f t="shared" ref="F115" si="31">E115/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G115">
         <v>10</v>
@@ -7003,14 +6982,13 @@
         <v>2.5</v>
       </c>
       <c r="D118">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E118">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F118">
-        <f t="shared" ref="F118" si="32">E118/10</f>
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G118">
         <v>10</v>
@@ -7049,8 +7027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
   <dimension ref="A1:G191"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -11579,7 +11557,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>